<commit_message>
Excel table of functionalities
</commit_message>
<xml_diff>
--- a/dokumenti/Excel table of functionalities.xlsx
+++ b/dokumenti/Excel table of functionalities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovan\Desktop\CineScreen\dokumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B692FCA1-3D53-416C-8E09-D5ABEDA0B656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB49083-0A9E-4A87-8F4C-4B7F9DA18912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>Učešće članova u implementaciji po funkcionalnostima</t>
   </si>
@@ -278,6 +277,45 @@
   </si>
   <si>
     <t>Movie, Projection, Genre, CinemaHall, MovieType, Seat</t>
+  </si>
+  <si>
+    <t>Multilanguage (i18n) implementacija po formi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prikaz slika </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Maps integracija </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carousel za prikaz proizvoda ili slika </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slajdšou (slideshow) prikaz slika </t>
+  </si>
+  <si>
+    <t>Lazy Loading for Angular Modules - update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP Interceptor in Angular for API Error Handling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsive Design with Angular </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Functionality with Debouncing in Angular </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full-Text Search </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Animations for UI Components </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multitenancy Support </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Obfuscation Techniques for Sensitive Information </t>
   </si>
 </sst>
 </file>
@@ -287,7 +325,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +403,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -516,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -607,6 +651,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -622,21 +681,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1346,32 +1391,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
     <col min="2" max="2" width="44.21875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.77734375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" style="7" customWidth="1"/>
     <col min="5" max="8" width="9.109375" style="1"/>
     <col min="9" max="9" width="1.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="1.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I5" s="9"/>
@@ -1390,57 +1435,57 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="33" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="25"/>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="35"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="40"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="38"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="35"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="40"/>
     </row>
     <row r="9" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
       <c r="B9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="21" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1524,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1531,7 +1576,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="6" t="s">
         <v>40</v>
       </c>
@@ -1579,7 +1624,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>41</v>
       </c>
@@ -1629,7 +1674,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1681,7 +1726,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="6" t="s">
         <v>43</v>
       </c>
@@ -1731,7 +1776,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="6" t="s">
         <v>44</v>
       </c>
@@ -1781,7 +1826,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="6" t="s">
         <v>45</v>
       </c>
@@ -1831,7 +1876,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="6" t="s">
         <v>46</v>
       </c>
@@ -1881,7 +1926,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="6" t="s">
         <v>47</v>
       </c>
@@ -1931,7 +1976,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="6" t="s">
         <v>48</v>
       </c>
@@ -1981,7 +2026,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="6" t="s">
         <v>49</v>
       </c>
@@ -2031,7 +2076,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="6" t="s">
         <v>50</v>
       </c>
@@ -2081,7 +2126,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="6" t="s">
         <v>51</v>
       </c>
@@ -2131,7 +2176,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="6" t="s">
         <v>52</v>
       </c>
@@ -2181,7 +2226,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="6" t="s">
         <v>53</v>
       </c>
@@ -2231,7 +2276,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="6" t="s">
         <v>54</v>
       </c>
@@ -2281,7 +2326,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="6" t="s">
         <v>55</v>
       </c>
@@ -2331,7 +2376,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="6" t="s">
         <v>56</v>
       </c>
@@ -2381,7 +2426,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="34" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -2433,7 +2478,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="6" t="s">
         <v>58</v>
       </c>
@@ -2483,7 +2528,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="6" t="s">
         <v>59</v>
       </c>
@@ -2533,7 +2578,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="6" t="s">
         <v>60</v>
       </c>
@@ -2583,7 +2628,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="6" t="s">
         <v>62</v>
       </c>
@@ -2633,7 +2678,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="6" t="s">
         <v>64</v>
       </c>
@@ -2683,7 +2728,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="6" t="s">
         <v>65</v>
       </c>
@@ -2733,7 +2778,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="6" t="s">
         <v>63</v>
       </c>
@@ -2783,12 +2828,12 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J36" s="32" t="s">
+      <c r="J36" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
       <c r="O36" s="16">
         <f>SUM(O10:O35)</f>
         <v>0</v>
@@ -2802,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
         <v>12</v>
       </c>
@@ -2822,168 +2867,213 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="26"/>
+      <c r="D40" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="26">
+        <v>4</v>
+      </c>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="26"/>
+      <c r="D41" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="26">
+        <v>3</v>
+      </c>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B42" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="26"/>
+      <c r="D42" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="26">
+        <v>5</v>
+      </c>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="26"/>
+      <c r="D43" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" s="26">
+        <v>3</v>
+      </c>
       <c r="F43" s="26"/>
       <c r="G43" s="26"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B44" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="26"/>
+      <c r="D44" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="26">
+        <v>3</v>
+      </c>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="26"/>
+      <c r="D45" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="26">
+        <v>5</v>
+      </c>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="26"/>
+      <c r="D46" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="26">
+        <v>3</v>
+      </c>
       <c r="F46" s="26"/>
       <c r="G46" s="26"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="26"/>
+      <c r="D47" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="26">
+        <v>5</v>
+      </c>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="26"/>
+      <c r="D48" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="26">
+        <v>3</v>
+      </c>
       <c r="F48" s="26"/>
       <c r="G48" s="26"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="26"/>
+      <c r="D49" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="26">
+        <v>6</v>
+      </c>
       <c r="F49" s="26"/>
       <c r="G49" s="26"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="26"/>
+      <c r="D50" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="26">
+        <v>3</v>
+      </c>
       <c r="F50" s="26"/>
       <c r="G50" s="26"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B51" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D51" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="28">
-        <f>SUM(E40:E50)</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="28">
-        <f>SUM(F40:F50)</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="28">
-        <f>SUM(G40:G50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D51" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="26">
+        <v>12</v>
+      </c>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D52" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="26">
+        <v>8</v>
+      </c>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
@@ -2992,6 +3082,10 @@
       <c r="B53" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
@@ -3000,6 +3094,10 @@
       <c r="B54" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
@@ -3008,6 +3106,21 @@
       <c r="B55" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D55" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="28">
+        <f>SUM(E40:E54)</f>
+        <v>63</v>
+      </c>
+      <c r="F55" s="28">
+        <f>SUM(F40:F50)</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="28">
+        <f>SUM(G40:G50)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
@@ -3016,6 +3129,18 @@
       <c r="B56" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D56" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
@@ -3063,16 +3188,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A27"/>
     <mergeCell ref="A28:A35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="E7:H8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="O8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="B40:B63">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">

</xml_diff>